<commit_message>
fix the error with relative paths
</commit_message>
<xml_diff>
--- a/src/backend_server/reports/report.xlsx
+++ b/src/backend_server/reports/report.xlsx
@@ -666,8 +666,12 @@
           <t>Магазин</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
       <c r="V2" t="n">
         <v>1</v>
       </c>
@@ -687,10 +691,10 @@
         <v>1</v>
       </c>
       <c r="AB2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
@@ -897,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X4" t="n">
         <v>1</v>
@@ -918,7 +922,7 @@
         <v>4</v>
       </c>
       <c r="AC4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -1025,22 +1029,22 @@
         <v>1</v>
       </c>
       <c r="X5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB5" t="n">
         <v>4</v>
       </c>
       <c r="AC5" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
@@ -1140,17 +1144,13 @@
       <c r="Y6" t="n">
         <v>1</v>
       </c>
-      <c r="Z6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>1</v>
-      </c>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="n">
         <v>2</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>4</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
@@ -1251,10 +1251,10 @@
         <v>2</v>
       </c>
       <c r="V7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X7" t="n">
         <v>1</v>
@@ -1268,11 +1268,11 @@
         <v>3</v>
       </c>
       <c r="AC7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Приоритет</t>
+          <t>Паритет</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add requests to classifier
</commit_message>
<xml_diff>
--- a/src/backend_server/reports/report.xlsx
+++ b/src/backend_server/reports/report.xlsx
@@ -667,38 +667,38 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
         <v>4</v>
       </c>
       <c r="AC2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Паритет</t>
+          <t>Диспаритет</t>
         </is>
       </c>
     </row>
@@ -895,34 +895,34 @@
         </is>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" t="n">
         <v>4</v>
       </c>
       <c r="AC4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -1017,38 +1017,38 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
         <v>4</v>
       </c>
       <c r="AC5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>Паритет</t>
+          <t>Диспаритет</t>
         </is>
       </c>
     </row>
@@ -1139,10 +1139,10 @@
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
@@ -1150,11 +1150,11 @@
         <v>1</v>
       </c>
       <c r="AC6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>Паритет</t>
+          <t>Диспаритет</t>
         </is>
       </c>
     </row>
@@ -1251,10 +1251,10 @@
         <v>2</v>
       </c>
       <c r="V7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X7" t="n">
         <v>1</v>
@@ -1268,7 +1268,7 @@
         <v>3</v>
       </c>
       <c r="AC7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>

</xml_diff>